<commit_message>
puerto rico field trip stuff (jan 2016 trip)
</commit_message>
<xml_diff>
--- a/PuertoRico-Field-Materials/Reimbursements/2015-Nov-PRtrip/reimbursement-tracking-2015-Nov-PRtrip.xlsx
+++ b/PuertoRico-Field-Materials/Reimbursements/2015-Nov-PRtrip/reimbursement-tracking-2015-Nov-PRtrip.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="11980" windowHeight="14560" tabRatio="500"/>
+    <workbookView xWindow="11700" yWindow="460" windowWidth="13900" windowHeight="14520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -172,12 +172,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -193,7 +199,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -202,6 +208,7 @@
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -484,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -499,49 +506,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
+      <c r="B1" s="9"/>
       <c r="C1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8"/>
+      <c r="B2" s="9"/>
       <c r="C2">
         <v>12840622</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="8"/>
+      <c r="B3" s="9"/>
       <c r="C3" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="9" t="s">
+      <c r="B4" s="9"/>
+      <c r="C4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5" s="9"/>
       <c r="C5" t="s">
         <v>23</v>
       </c>
@@ -551,10 +558,10 @@
       <c r="B6" s="6"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="8"/>
+      <c r="B7" s="9"/>
       <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
@@ -569,10 +576,10 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="8"/>
+      <c r="B8" s="9"/>
       <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
@@ -637,9 +644,11 @@
       <c r="B16" t="s">
         <v>25</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="8">
         <v>201.3</v>
       </c>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
@@ -648,9 +657,11 @@
       <c r="B17" t="s">
         <v>28</v>
       </c>
-      <c r="E17">
+      <c r="D17" s="8"/>
+      <c r="E17" s="8">
         <v>40</v>
       </c>
+      <c r="F17" s="8"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
@@ -659,7 +670,9 @@
       <c r="B18" t="s">
         <v>27</v>
       </c>
-      <c r="F18">
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8">
         <v>60</v>
       </c>
     </row>
@@ -758,7 +771,7 @@
       <c r="B27" t="s">
         <v>34</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="8">
         <v>44.3</v>
       </c>
     </row>
@@ -769,8 +782,26 @@
       <c r="B28" t="s">
         <v>35</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="8">
         <v>148.18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I31">
+        <f>SUM(I19:I26)</f>
+        <v>297.51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D32">
+        <f>SUM(D16:D31)</f>
+        <v>349.48</v>
+      </c>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F34">
+        <f>SUM(D16:F28)</f>
+        <v>493.78000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
filing reimbursements for field work
</commit_message>
<xml_diff>
--- a/PuertoRico-Field-Materials/Reimbursements/2015-Nov-PRtrip/reimbursement-tracking-2015-Nov-PRtrip.xlsx
+++ b/PuertoRico-Field-Materials/Reimbursements/2015-Nov-PRtrip/reimbursement-tracking-2015-Nov-PRtrip.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t>Name</t>
   </si>
@@ -132,6 +132,12 @@
   </si>
   <si>
     <t>Flight SJU to BWI (JetBlue)</t>
+  </si>
+  <si>
+    <t>Hardware supplies for Puerto Rico field work</t>
+  </si>
+  <si>
+    <t>electrical supplies for Puerto Rico field work</t>
   </si>
 </sst>
 </file>
@@ -491,18 +497,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" topLeftCell="C3" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="33.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="5" width="10.83203125" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" customWidth="1"/>
+    <col min="7" max="8" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -650,7 +658,7 @@
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
         <v>42311</v>
       </c>
@@ -663,7 +671,7 @@
       </c>
       <c r="F17" s="8"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
         <v>42311</v>
       </c>
@@ -676,95 +684,109 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
         <v>42310</v>
       </c>
       <c r="B19" t="s">
         <v>26</v>
       </c>
-      <c r="I19">
-        <v>50.79</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I19" s="8">
+        <v>50.97</v>
+      </c>
+      <c r="K19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
         <v>42311</v>
       </c>
       <c r="B20" t="s">
         <v>26</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="8">
         <v>34.46</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K20">
+        <f>SUM(I19:I21,I23,)</f>
+        <v>164.73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
         <v>42314</v>
       </c>
       <c r="B21" t="s">
         <v>29</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="8">
         <v>74.27</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="7">
         <v>42320</v>
       </c>
       <c r="B22" t="s">
         <v>30</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="8">
         <v>41.84</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="7">
         <v>42320</v>
       </c>
       <c r="B23" t="s">
         <v>31</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="8">
         <v>5.03</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K23">
+        <f>SUM(I22,I24,I25,I26)</f>
+        <v>132.96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="7">
         <v>42320</v>
       </c>
       <c r="B24" t="s">
         <v>32</v>
       </c>
-      <c r="I24">
+      <c r="I24" s="8">
         <v>16.71</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="7">
         <v>42338</v>
       </c>
       <c r="B25" t="s">
         <v>30</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="8">
         <v>29.88</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="7">
         <v>42342</v>
       </c>
       <c r="B26" t="s">
         <v>33</v>
       </c>
-      <c r="I26">
+      <c r="I26" s="8">
         <v>44.53</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="7">
         <v>42348</v>
       </c>
@@ -775,7 +797,7 @@
         <v>44.3</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="7">
         <v>42341</v>
       </c>
@@ -786,13 +808,13 @@
         <v>148.18</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="I31">
         <f>SUM(I19:I26)</f>
-        <v>297.51</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+        <v>297.69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D32">
         <f>SUM(D16:D31)</f>
         <v>349.48</v>

</xml_diff>